<commit_message>
Training and test files swapped
</commit_message>
<xml_diff>
--- a/k-nnClassifier/graph.xlsx
+++ b/k-nnClassifier/graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\4 sem\NAI\k-nnClassifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{239FC182-32EB-4B05-857C-7520130A9837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6E320C-76AE-460E-B034-243F411AF70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{054D63EB-0EE9-4C5B-94A4-9216EE90CB4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{054D63EB-0EE9-4C5B-94A4-9216EE90CB4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>